<commit_message>
calculated installemts using the PMT function
</commit_message>
<xml_diff>
--- a/Loan Management System.xlsx
+++ b/Loan Management System.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ms Konya\Downloads\Fablab -Data Analytics and visualization\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ms Konya\Downloads\Fablab -Data Analytics and visualization\Excel\LoanManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29721ADE-9E6F-40A8-A50F-9ABE44CC6943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CDD43E-B877-44A1-9C7B-0FDCBEF8CD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D45ECFA9-0EF8-446D-AF0B-F9EF2BA9B9A2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="83">
   <si>
     <t>MemberID</t>
   </si>
@@ -301,11 +301,17 @@
   <si>
     <t>Total loan Taken</t>
   </si>
+  <si>
+    <t>Installment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -393,17 +399,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78AF8D1-B484-497E-9163-B0A68CAA0D33}">
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="N10" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,30 +779,31 @@
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -843,12 +851,12 @@
       <c r="Q2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -861,18 +869,18 @@
         <v>45292</v>
       </c>
       <c r="D3">
-        <f ca="1">DATEDIF($C3,$B$24,"YM")</f>
+        <f t="shared" ref="D3:D22" ca="1" si="0">DATEDIF($C3,$B$24,"YM")</f>
         <v>6</v>
       </c>
       <c r="E3">
-        <f ca="1">$D3*4</f>
+        <f t="shared" ref="E3:E22" ca="1" si="1">$D3*4</f>
         <v>24</v>
       </c>
       <c r="F3">
         <v>1523</v>
       </c>
       <c r="G3">
-        <f ca="1">$E3*$F3</f>
+        <f t="shared" ref="G3:G22" ca="1" si="2">$E3*$F3</f>
         <v>36552</v>
       </c>
       <c r="H3">
@@ -888,13 +896,13 @@
       <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="10">
         <v>0.22</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="11">
         <f>$O3/12</f>
         <v>1.8333333333333333E-2</v>
       </c>
@@ -928,22 +936,22 @@
         <v>45292</v>
       </c>
       <c r="D4">
-        <f ca="1">DATEDIF($C4,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E4">
-        <f ca="1">$D4*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F4">
         <v>4370</v>
       </c>
       <c r="G4">
-        <f ca="1">$E4*$F4</f>
+        <f t="shared" ca="1" si="2"/>
         <v>104880</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:J22" ca="1" si="0">$G4*3</f>
+        <f t="shared" ref="H4:H22" ca="1" si="3">$G4*3</f>
         <v>314640</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -955,13 +963,13 @@
       <c r="M4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="10">
         <v>0.21</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="11">
         <f>$O4/12</f>
         <v>1.7499999999999998E-2</v>
       </c>
@@ -974,7 +982,7 @@
       <c r="U4" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="12">
+      <c r="W4" s="10">
         <v>0.2</v>
       </c>
     </row>
@@ -989,22 +997,22 @@
         <v>45292</v>
       </c>
       <c r="D5">
-        <f ca="1">DATEDIF($C5,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E5">
-        <f ca="1">$D5*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F5">
         <v>4880</v>
       </c>
       <c r="G5">
-        <f ca="1">$E5*$F5</f>
+        <f t="shared" ca="1" si="2"/>
         <v>117120</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>351360</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -1016,13 +1024,13 @@
       <c r="M5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="10">
         <v>0.23</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="11">
         <f>$O5/12</f>
         <v>1.9166666666666669E-2</v>
       </c>
@@ -1035,7 +1043,7 @@
       <c r="U5" t="s">
         <v>27</v>
       </c>
-      <c r="W5" s="12">
+      <c r="W5" s="10">
         <v>0.2</v>
       </c>
     </row>
@@ -1050,22 +1058,22 @@
         <v>45292</v>
       </c>
       <c r="D6">
-        <f ca="1">DATEDIF($C6,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E6">
-        <f ca="1">$D6*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F6">
         <v>3656</v>
       </c>
       <c r="G6">
-        <f ca="1">$E6*$F6</f>
+        <f t="shared" ca="1" si="2"/>
         <v>87744</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>263232</v>
       </c>
       <c r="I6" s="8" t="s">
@@ -1077,13 +1085,13 @@
       <c r="M6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="11">
         <f>$O6/12</f>
         <v>1.1666666666666667E-2</v>
       </c>
@@ -1102,22 +1110,22 @@
         <v>45292</v>
       </c>
       <c r="D7">
-        <f ca="1">DATEDIF($C7,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E7">
-        <f ca="1">$D7*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F7">
         <v>2818</v>
       </c>
       <c r="G7">
-        <f ca="1">$E7*$F7</f>
+        <f t="shared" ca="1" si="2"/>
         <v>67632</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>202896</v>
       </c>
       <c r="I7" s="8" t="s">
@@ -1129,7 +1137,7 @@
       <c r="M7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="O7" t="s">
@@ -1153,22 +1161,22 @@
         <v>45292</v>
       </c>
       <c r="D8">
-        <f ca="1">DATEDIF($C8,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E8">
-        <f ca="1">$D8*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F8">
         <v>2868</v>
       </c>
       <c r="G8">
-        <f ca="1">$E8*$F8</f>
+        <f t="shared" ca="1" si="2"/>
         <v>68832</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>206496</v>
       </c>
       <c r="I8" s="8" t="s">
@@ -1190,22 +1198,22 @@
         <v>45292</v>
       </c>
       <c r="D9">
-        <f ca="1">DATEDIF($C9,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E9">
-        <f ca="1">$D9*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F9">
         <v>3623</v>
       </c>
       <c r="G9">
-        <f ca="1">$E9*$F9</f>
+        <f t="shared" ca="1" si="2"/>
         <v>86952</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>260856</v>
       </c>
       <c r="I9" s="8" t="s">
@@ -1231,35 +1239,35 @@
         <v>45292</v>
       </c>
       <c r="D10">
-        <f ca="1">DATEDIF($C10,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E10">
-        <f ca="1">$D10*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F10">
         <v>2562</v>
       </c>
       <c r="G10">
-        <f ca="1">$E10*$F10</f>
+        <f t="shared" ca="1" si="2"/>
         <v>61488</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>184464</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="14">
         <v>17000</v>
       </c>
       <c r="V10" s="1"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1272,22 +1280,22 @@
         <v>45292</v>
       </c>
       <c r="D11">
-        <f ca="1">DATEDIF($C11,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E11">
-        <f ca="1">$D11*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F11">
         <v>1457</v>
       </c>
       <c r="G11">
-        <f ca="1">$E11*$F11</f>
+        <f t="shared" ca="1" si="2"/>
         <v>34968</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>104904</v>
       </c>
       <c r="I11" s="8" t="s">
@@ -1296,10 +1304,10 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1312,22 +1320,22 @@
         <v>45292</v>
       </c>
       <c r="D12">
-        <f ca="1">DATEDIF($C12,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E12">
-        <f ca="1">$D12*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F12">
         <v>1555</v>
       </c>
       <c r="G12">
-        <f ca="1">$E12*$F12</f>
+        <f t="shared" ca="1" si="2"/>
         <v>37320</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>111960</v>
       </c>
       <c r="I12" s="8" t="s">
@@ -1353,6 +1361,9 @@
       </c>
       <c r="R12" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="V12" s="1"/>
     </row>
@@ -1367,35 +1378,35 @@
         <v>45292</v>
       </c>
       <c r="D13">
-        <f ca="1">DATEDIF($C13,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E13">
-        <f ca="1">$D13*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F13">
         <v>1625</v>
       </c>
       <c r="G13">
-        <f ca="1">$E13*$F13</f>
+        <f t="shared" ca="1" si="2"/>
         <v>39000</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>117000</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="13">
         <v>100000</v>
       </c>
       <c r="M13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="N13" t="str">
-        <f>VLOOKUP($M13,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" ref="N13:N19" si="4">VLOOKUP($M13,$A$3:$I$22,9,FALSE)</f>
         <v>L02</v>
       </c>
       <c r="O13">
@@ -1405,7 +1416,7 @@
       <c r="P13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="11">
         <f>VLOOKUP($P13,$M$2:$Q$7,4,FALSE)</f>
         <v>1.7499999999999998E-2</v>
       </c>
@@ -1413,6 +1424,10 @@
         <f>VLOOKUP($P13,$M$2:$Q$7,5,FALSE)</f>
         <v>15</v>
       </c>
+      <c r="S13" s="17">
+        <f>-PMT($Q13,$R13,$O13)</f>
+        <v>24031.381096417233</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1425,22 +1440,22 @@
         <v>45292</v>
       </c>
       <c r="D14">
-        <f ca="1">DATEDIF($C14,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E14">
-        <f ca="1">$D14*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F14">
         <v>2490</v>
       </c>
       <c r="G14">
-        <f ca="1">$E14*$F14</f>
+        <f t="shared" ca="1" si="2"/>
         <v>59760</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>179280</v>
       </c>
       <c r="I14" s="8" t="s">
@@ -1453,23 +1468,27 @@
         <v>12</v>
       </c>
       <c r="N14" t="str">
-        <f>VLOOKUP($M14,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>L01</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14:O19" si="1">VLOOKUP($M14,$A$3:$J$24,10,FALSE)</f>
+        <f t="shared" ref="O14:O19" si="5">VLOOKUP($M14,$A$3:$J$24,10,FALSE)</f>
         <v>17000</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Q14" s="13">
-        <f t="shared" ref="Q14:Q19" si="2">VLOOKUP($P14,$M$2:$Q$7,4,FALSE)</f>
+      <c r="Q14" s="11">
+        <f t="shared" ref="Q14:Q19" si="6">VLOOKUP($P14,$M$2:$Q$7,4,FALSE)</f>
         <v>1.8333333333333333E-2</v>
       </c>
       <c r="R14">
-        <f t="shared" ref="R14:R19" si="3">VLOOKUP($P14,$M$2:$Q$7,5,FALSE)</f>
+        <f t="shared" ref="R14:R19" si="7">VLOOKUP($P14,$M$2:$Q$7,5,FALSE)</f>
         <v>24</v>
+      </c>
+      <c r="S14" s="17">
+        <f t="shared" ref="S14:S19" si="8">-PMT($Q14,$R14,$O14)</f>
+        <v>881.92862901150772</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -1483,18 +1502,18 @@
         <v>45292</v>
       </c>
       <c r="D15">
-        <f ca="1">DATEDIF($C15,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="E15">
-        <f ca="1">$D15*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="F15">
         <v>3080</v>
       </c>
       <c r="G15">
-        <f ca="1">$E15*$F15</f>
+        <f t="shared" ca="1" si="2"/>
         <v>73920</v>
       </c>
       <c r="H15">
@@ -1504,30 +1523,34 @@
       <c r="I15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="13">
         <v>22000</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N15" t="str">
-        <f>VLOOKUP($M15,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>L04</v>
       </c>
       <c r="O15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>100000</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="13">
-        <f t="shared" si="2"/>
+      <c r="Q15" s="11">
+        <f t="shared" si="6"/>
         <v>1.1666666666666667E-2</v>
       </c>
       <c r="R15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>20</v>
+      </c>
+      <c r="S15" s="17">
+        <f t="shared" si="8"/>
+        <v>5634.9772872595904</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -1541,22 +1564,22 @@
         <v>45323</v>
       </c>
       <c r="D16">
-        <f ca="1">DATEDIF($C16,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E16">
-        <f ca="1">$D16*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F16">
         <v>714</v>
       </c>
       <c r="G16">
-        <f ca="1">$E16*$F16</f>
+        <f t="shared" ca="1" si="2"/>
         <v>14280</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>42840</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -1569,26 +1592,30 @@
         <v>17</v>
       </c>
       <c r="N16" t="str">
-        <f>VLOOKUP($M16,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>L03</v>
       </c>
       <c r="O16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>22000</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q16" s="13">
-        <f t="shared" si="2"/>
+      <c r="Q16" s="11">
+        <f t="shared" si="6"/>
         <v>1.9166666666666669E-2</v>
       </c>
       <c r="R16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="17">
+        <f t="shared" si="8"/>
+        <v>2069.6790693834346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1599,22 +1626,22 @@
         <v>45323</v>
       </c>
       <c r="D17">
-        <f ca="1">DATEDIF($C17,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E17">
-        <f ca="1">$D17*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F17">
         <v>1552</v>
       </c>
       <c r="G17">
-        <f ca="1">$E17*$F17</f>
+        <f t="shared" ca="1" si="2"/>
         <v>31040</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>93120</v>
       </c>
       <c r="I17" s="8" t="s">
@@ -1627,26 +1654,30 @@
         <v>20</v>
       </c>
       <c r="N17" t="str">
-        <f>VLOOKUP($M17,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>L04</v>
       </c>
       <c r="O17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>269280</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q17" s="13">
-        <f t="shared" si="2"/>
+      <c r="Q17" s="11">
+        <f t="shared" si="6"/>
         <v>1.1666666666666667E-2</v>
       </c>
       <c r="R17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="17">
+        <f t="shared" si="8"/>
+        <v>15173.866839132623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1657,22 +1688,22 @@
         <v>45323</v>
       </c>
       <c r="D18">
-        <f ca="1">DATEDIF($C18,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E18">
-        <f ca="1">$D18*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F18">
         <v>4488</v>
       </c>
       <c r="G18">
-        <f ca="1">$E18*$F18</f>
+        <f t="shared" ca="1" si="2"/>
         <v>89760</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>269280</v>
       </c>
       <c r="I18" s="8" t="s">
@@ -1685,26 +1716,30 @@
         <v>21</v>
       </c>
       <c r="N18" t="str">
-        <f>VLOOKUP($M18,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>L03</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>168480</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="13">
-        <f t="shared" si="2"/>
+      <c r="Q18" s="11">
+        <f t="shared" si="6"/>
         <v>1.9166666666666669E-2</v>
       </c>
       <c r="R18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="17">
+        <f t="shared" si="8"/>
+        <v>15849.978618623683</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1715,22 +1750,22 @@
         <v>45323</v>
       </c>
       <c r="D19">
-        <f ca="1">DATEDIF($C19,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E19">
-        <f ca="1">$D19*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F19">
         <v>2808</v>
       </c>
       <c r="G19">
-        <f ca="1">$E19*$F19</f>
+        <f t="shared" ca="1" si="2"/>
         <v>56160</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>168480</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -1743,26 +1778,30 @@
         <v>24</v>
       </c>
       <c r="N19" t="str">
-        <f>VLOOKUP($M19,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>L03</v>
       </c>
       <c r="O19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>190140</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q19" s="13">
-        <f t="shared" si="2"/>
+      <c r="Q19" s="11">
+        <f t="shared" si="6"/>
         <v>1.9166666666666669E-2</v>
       </c>
       <c r="R19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="17">
+        <f t="shared" si="8"/>
+        <v>17887.671738753012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1773,22 +1812,22 @@
         <v>45323</v>
       </c>
       <c r="D20">
-        <f ca="1">DATEDIF($C20,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E20">
-        <f ca="1">$D20*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F20">
         <v>1988</v>
       </c>
       <c r="G20">
-        <f ca="1">$E20*$F20</f>
+        <f t="shared" ca="1" si="2"/>
         <v>39760</v>
       </c>
       <c r="H20">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>119280</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -1799,7 +1838,7 @@
       </c>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1810,22 +1849,22 @@
         <v>45323</v>
       </c>
       <c r="D21">
-        <f ca="1">DATEDIF($C21,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E21">
-        <f ca="1">$D21*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F21">
         <v>4770</v>
       </c>
       <c r="G21">
-        <f ca="1">$E21*$F21</f>
+        <f t="shared" ca="1" si="2"/>
         <v>95400</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>286200</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -1835,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1846,22 +1885,22 @@
         <v>45323</v>
       </c>
       <c r="D22">
-        <f ca="1">DATEDIF($C22,$B$24,"YM")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E22">
-        <f ca="1">$D22*4</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="F22">
         <v>3169</v>
       </c>
       <c r="G22">
-        <f ca="1">$E22*$F22</f>
+        <f t="shared" ca="1" si="2"/>
         <v>63380</v>
       </c>
       <c r="H22">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="3"/>
         <v>190140</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -1871,7 +1910,7 @@
         <v>190140</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1881,7 +1920,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
@@ -1891,7 +1930,7 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1914,37 +1953,44 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>6</v>
+      </c>
       <c r="M26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <f>VLOOKUP(L26,A3:J22,10,FALSE)</f>
+        <v>314640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M31">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M32">
         <v>7</v>
       </c>
@@ -1960,11 +2006,11 @@
       </c>
     </row>
     <row r="34" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
       <c r="M34">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
added a loan amoutanization table
</commit_message>
<xml_diff>
--- a/Loan Management System.xlsx
+++ b/Loan Management System.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ms Konya\Downloads\Fablab -Data Analytics and visualization\Excel\LoanManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CDD43E-B877-44A1-9C7B-0FDCBEF8CD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A33C70-6AE1-4D3B-8E4C-9D844FFEC33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D45ECFA9-0EF8-446D-AF0B-F9EF2BA9B9A2}"/>
   </bookViews>
@@ -382,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -411,6 +411,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78AF8D1-B484-497E-9163-B0A68CAA0D33}">
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N10" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +780,7 @@
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
   </cols>
@@ -1406,7 +1407,7 @@
         <v>6</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" ref="N13:N19" si="4">VLOOKUP($M13,$A$3:$I$22,9,FALSE)</f>
+        <f t="shared" ref="N13:N20" si="4">VLOOKUP($M13,$A$3:$I$22,9,FALSE)</f>
         <v>L02</v>
       </c>
       <c r="O13">
@@ -1472,22 +1473,22 @@
         <v>L01</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14:O19" si="5">VLOOKUP($M14,$A$3:$J$24,10,FALSE)</f>
+        <f t="shared" ref="O14:O20" si="5">VLOOKUP($M14,$A$3:$J$24,10,FALSE)</f>
         <v>17000</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>32</v>
       </c>
       <c r="Q14" s="11">
-        <f t="shared" ref="Q14:Q19" si="6">VLOOKUP($P14,$M$2:$Q$7,4,FALSE)</f>
+        <f t="shared" ref="Q14:Q20" si="6">VLOOKUP($P14,$M$2:$Q$7,4,FALSE)</f>
         <v>1.8333333333333333E-2</v>
       </c>
       <c r="R14">
-        <f t="shared" ref="R14:R19" si="7">VLOOKUP($P14,$M$2:$Q$7,5,FALSE)</f>
+        <f t="shared" ref="R14:R20" si="7">VLOOKUP($P14,$M$2:$Q$7,5,FALSE)</f>
         <v>24</v>
       </c>
       <c r="S14" s="17">
-        <f t="shared" ref="S14:S19" si="8">-PMT($Q14,$R14,$O14)</f>
+        <f t="shared" ref="S14:S20" si="8">-PMT($Q14,$R14,$O14)</f>
         <v>881.92862901150772</v>
       </c>
     </row>
@@ -1837,6 +1838,8 @@
         <v>0</v>
       </c>
       <c r="M20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1955,25 +1958,39 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L26" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26">
         <f>VLOOKUP(L26,A3:J22,10,FALSE)</f>
-        <v>314640</v>
+        <v>168480</v>
+      </c>
+      <c r="O26" s="17">
+        <f>VLOOKUP(L26,M13:S19,7,FALSE)</f>
+        <v>15849.978618623683</v>
+      </c>
+      <c r="P26" s="18">
+        <f>VLOOKUP(L26,M13:S19,5,FALSE)*N26</f>
+        <v>3229.2000000000003</v>
+      </c>
+      <c r="Q26" s="17">
+        <f>O26-P26</f>
+        <v>12620.778618623683</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M27">
         <v>2</v>
       </c>
+      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M28">
         <v>3</v>
       </c>
+      <c r="O28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M29">
@@ -2116,7 +2133,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I23" xr:uid="{59038AD0-06A5-45B2-A516-1150ACDC566C}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P12:P19" xr:uid="{CCE4B299-799C-49F8-9BF3-74844DA3BD82}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P12:P20" xr:uid="{CCE4B299-799C-49F8-9BF3-74844DA3BD82}">
       <formula1>$M$3:$M$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Completed Loan Amoutization table
</commit_message>
<xml_diff>
--- a/Loan Management System.xlsx
+++ b/Loan Management System.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ms Konya\Downloads\Fablab -Data Analytics and visualization\Excel\LoanManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A33C70-6AE1-4D3B-8E4C-9D844FFEC33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB53E74-46FE-4E71-8C7E-607B6E87273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D45ECFA9-0EF8-446D-AF0B-F9EF2BA9B9A2}"/>
   </bookViews>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78AF8D1-B484-497E-9163-B0A68CAA0D33}">
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,62 +1957,184 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L26" t="s">
-        <v>21</v>
+      <c r="L26" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26">
         <f>VLOOKUP(L26,A3:J22,10,FALSE)</f>
-        <v>168480</v>
+        <v>269280</v>
       </c>
       <c r="O26" s="17">
-        <f>VLOOKUP(L26,M13:S19,7,FALSE)</f>
-        <v>15849.978618623683</v>
+        <f>VLOOKUP($L26,$M$13:$S$19,7,FALSE)</f>
+        <v>15173.866839132623</v>
       </c>
       <c r="P26" s="18">
-        <f>VLOOKUP(L26,M13:S19,5,FALSE)*N26</f>
-        <v>3229.2000000000003</v>
-      </c>
-      <c r="Q26" s="17">
+        <f>VLOOKUP($L26,$M$13:$S$19,5,FALSE)*N26</f>
+        <v>3141.6000000000004</v>
+      </c>
+      <c r="Q26" s="18">
         <f>O26-P26</f>
-        <v>12620.778618623683</v>
+        <v>12032.266839132622</v>
+      </c>
+      <c r="R26" s="17">
+        <f>N26-Q26</f>
+        <v>257247.73316086738</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M27">
         <v>2</v>
       </c>
-      <c r="O27" s="17"/>
+      <c r="N27" s="17">
+        <f>$R26</f>
+        <v>257247.73316086738</v>
+      </c>
+      <c r="O27" s="17">
+        <f>$O$26</f>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P27" s="18">
+        <f>VLOOKUP($L$26,$M$13:$S$19,5,FALSE)*$N27</f>
+        <v>3001.2235535434529</v>
+      </c>
+      <c r="Q27" s="17">
+        <f>$O$27-$P27</f>
+        <v>12172.643285589169</v>
+      </c>
+      <c r="R27" s="17">
+        <f>$N27-$Q27</f>
+        <v>245075.08987527821</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M28">
         <v>3</v>
       </c>
-      <c r="O28" s="17"/>
+      <c r="N28" s="17">
+        <f t="shared" ref="N28:N45" si="9">$R27</f>
+        <v>245075.08987527821</v>
+      </c>
+      <c r="O28" s="17">
+        <f t="shared" ref="O28:O45" si="10">$O$26</f>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P28" s="18">
+        <f t="shared" ref="P28:P45" si="11">VLOOKUP($L$26,$M$13:$S$19,5,FALSE)*$N28</f>
+        <v>2859.2093818782459</v>
+      </c>
+      <c r="Q28" s="17">
+        <f t="shared" ref="Q28:Q45" si="12">$O$27-$P28</f>
+        <v>12314.657457254376</v>
+      </c>
+      <c r="R28" s="17">
+        <f t="shared" ref="R28:R45" si="13">$N28-$Q28</f>
+        <v>232760.43241802382</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M29">
         <v>4</v>
       </c>
+      <c r="N29" s="17">
+        <f t="shared" si="9"/>
+        <v>232760.43241802382</v>
+      </c>
+      <c r="O29" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P29" s="18">
+        <f t="shared" si="11"/>
+        <v>2715.5383782102781</v>
+      </c>
+      <c r="Q29" s="17">
+        <f t="shared" si="12"/>
+        <v>12458.328460922345</v>
+      </c>
+      <c r="R29" s="17">
+        <f t="shared" si="13"/>
+        <v>220302.10395710147</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M30">
         <v>5</v>
       </c>
+      <c r="N30" s="17">
+        <f t="shared" si="9"/>
+        <v>220302.10395710147</v>
+      </c>
+      <c r="O30" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P30" s="18">
+        <f t="shared" si="11"/>
+        <v>2570.1912128328504</v>
+      </c>
+      <c r="Q30" s="17">
+        <f t="shared" si="12"/>
+        <v>12603.675626299773</v>
+      </c>
+      <c r="R30" s="17">
+        <f t="shared" si="13"/>
+        <v>207698.42833080169</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M31">
         <v>6</v>
       </c>
+      <c r="N31" s="17">
+        <f t="shared" si="9"/>
+        <v>207698.42833080169</v>
+      </c>
+      <c r="O31" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P31" s="18">
+        <f t="shared" si="11"/>
+        <v>2423.1483305260199</v>
+      </c>
+      <c r="Q31" s="17">
+        <f t="shared" si="12"/>
+        <v>12750.718508606602</v>
+      </c>
+      <c r="R31" s="17">
+        <f t="shared" si="13"/>
+        <v>194947.70982219509</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M32">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="17">
+        <f t="shared" si="9"/>
+        <v>194947.70982219509</v>
+      </c>
+      <c r="O32" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P32" s="18">
+        <f t="shared" si="11"/>
+        <v>2274.3899479256092</v>
+      </c>
+      <c r="Q32" s="17">
+        <f t="shared" si="12"/>
+        <v>12899.476891207014</v>
+      </c>
+      <c r="R32" s="17">
+        <f t="shared" si="13"/>
+        <v>182048.23293098807</v>
+      </c>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2021,8 +2143,28 @@
       <c r="M33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="17">
+        <f t="shared" si="9"/>
+        <v>182048.23293098807</v>
+      </c>
+      <c r="O33" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P33" s="18">
+        <f t="shared" si="11"/>
+        <v>2123.8960508615278</v>
+      </c>
+      <c r="Q33" s="17">
+        <f t="shared" si="12"/>
+        <v>13049.970788271095</v>
+      </c>
+      <c r="R33" s="17">
+        <f t="shared" si="13"/>
+        <v>168998.26214271697</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
@@ -2031,81 +2173,341 @@
       <c r="M34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="17">
+        <f t="shared" si="9"/>
+        <v>168998.26214271697</v>
+      </c>
+      <c r="O34" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P34" s="18">
+        <f t="shared" si="11"/>
+        <v>1971.6463916650314</v>
+      </c>
+      <c r="Q34" s="17">
+        <f t="shared" si="12"/>
+        <v>13202.220447467591</v>
+      </c>
+      <c r="R34" s="17">
+        <f t="shared" si="13"/>
+        <v>155796.04169524938</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="17">
+        <f t="shared" si="9"/>
+        <v>155796.04169524938</v>
+      </c>
+      <c r="O35" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P35" s="18">
+        <f t="shared" si="11"/>
+        <v>1817.6204864445763</v>
+      </c>
+      <c r="Q35" s="17">
+        <f t="shared" si="12"/>
+        <v>13356.246352688046</v>
+      </c>
+      <c r="R35" s="17">
+        <f t="shared" si="13"/>
+        <v>142439.79534256132</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="17">
+        <f t="shared" si="9"/>
+        <v>142439.79534256132</v>
+      </c>
+      <c r="O36" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P36" s="18">
+        <f t="shared" si="11"/>
+        <v>1661.7976123298822</v>
+      </c>
+      <c r="Q36" s="17">
+        <f t="shared" si="12"/>
+        <v>13512.069226802741</v>
+      </c>
+      <c r="R36" s="17">
+        <f t="shared" si="13"/>
+        <v>128927.72611575859</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M37">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="17">
+        <f t="shared" si="9"/>
+        <v>128927.72611575859</v>
+      </c>
+      <c r="O37" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P37" s="18">
+        <f t="shared" si="11"/>
+        <v>1504.1568046838502</v>
+      </c>
+      <c r="Q37" s="17">
+        <f t="shared" si="12"/>
+        <v>13669.710034448774</v>
+      </c>
+      <c r="R37" s="17">
+        <f t="shared" si="13"/>
+        <v>115258.01608130982</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="17">
+        <f t="shared" si="9"/>
+        <v>115258.01608130982</v>
+      </c>
+      <c r="O38" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P38" s="18">
+        <f t="shared" si="11"/>
+        <v>1344.676854281948</v>
+      </c>
+      <c r="Q38" s="17">
+        <f t="shared" si="12"/>
+        <v>13829.189984850675</v>
+      </c>
+      <c r="R38" s="17">
+        <f t="shared" si="13"/>
+        <v>101428.82609645915</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M39">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="17">
+        <f t="shared" si="9"/>
+        <v>101428.82609645915</v>
+      </c>
+      <c r="O39" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P39" s="18">
+        <f t="shared" si="11"/>
+        <v>1183.3363044586902</v>
+      </c>
+      <c r="Q39" s="17">
+        <f t="shared" si="12"/>
+        <v>13990.530534673933</v>
+      </c>
+      <c r="R39" s="17">
+        <f t="shared" si="13"/>
+        <v>87438.295561785213</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M40">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="17">
+        <f t="shared" si="9"/>
+        <v>87438.295561785213</v>
+      </c>
+      <c r="O40" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P40" s="18">
+        <f t="shared" si="11"/>
+        <v>1020.1134482208275</v>
+      </c>
+      <c r="Q40" s="17">
+        <f t="shared" si="12"/>
+        <v>14153.753390911796</v>
+      </c>
+      <c r="R40" s="17">
+        <f t="shared" si="13"/>
+        <v>73284.542170873421</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M41">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="17">
+        <f t="shared" si="9"/>
+        <v>73284.542170873421</v>
+      </c>
+      <c r="O41" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P41" s="18">
+        <f t="shared" si="11"/>
+        <v>854.98632532685667</v>
+      </c>
+      <c r="Q41" s="17">
+        <f t="shared" si="12"/>
+        <v>14318.880513805767</v>
+      </c>
+      <c r="R41" s="17">
+        <f t="shared" si="13"/>
+        <v>58965.661657067656</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M42">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="17">
+        <f t="shared" si="9"/>
+        <v>58965.661657067656</v>
+      </c>
+      <c r="O42" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P42" s="18">
+        <f t="shared" si="11"/>
+        <v>687.93271933245603</v>
+      </c>
+      <c r="Q42" s="17">
+        <f t="shared" si="12"/>
+        <v>14485.934119800168</v>
+      </c>
+      <c r="R42" s="17">
+        <f t="shared" si="13"/>
+        <v>44479.727537267492</v>
+      </c>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M43">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="17">
+        <f t="shared" si="9"/>
+        <v>44479.727537267492</v>
+      </c>
+      <c r="O43" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P43" s="18">
+        <f t="shared" si="11"/>
+        <v>518.93015460145409</v>
+      </c>
+      <c r="Q43" s="17">
+        <f t="shared" si="12"/>
+        <v>14654.936684531169</v>
+      </c>
+      <c r="R43" s="17">
+        <f t="shared" si="13"/>
+        <v>29824.790852736325</v>
+      </c>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M44">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="17">
+        <f t="shared" si="9"/>
+        <v>29824.790852736325</v>
+      </c>
+      <c r="O44" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P44" s="18">
+        <f t="shared" si="11"/>
+        <v>347.95589328192381</v>
+      </c>
+      <c r="Q44" s="17">
+        <f t="shared" si="12"/>
+        <v>14825.910945850699</v>
+      </c>
+      <c r="R44" s="17">
+        <f t="shared" si="13"/>
+        <v>14998.879906885626</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M45">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="17">
+        <f t="shared" si="9"/>
+        <v>14998.879906885626</v>
+      </c>
+      <c r="O45" s="17">
+        <f t="shared" si="10"/>
+        <v>15173.866839132623</v>
+      </c>
+      <c r="P45" s="18">
+        <f t="shared" si="11"/>
+        <v>174.98693224699898</v>
+      </c>
+      <c r="Q45" s="17">
+        <f t="shared" si="12"/>
+        <v>14998.879906885624</v>
+      </c>
+      <c r="R45" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M46">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M47">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M48">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+    </row>
+    <row r="49" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M49">
         <v>24</v>
       </c>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2127,7 +2529,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M20" xr:uid="{58C9453E-810E-46A2-9140-433AE25A9689}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M20 L25:L26" xr:uid="{58C9453E-810E-46A2-9140-433AE25A9689}">
       <formula1>$A$3:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I23" xr:uid="{59038AD0-06A5-45B2-A516-1150ACDC566C}">

</xml_diff>